<commit_message>
Thats a productive day for sure 💯
I'm loving the process .
</commit_message>
<xml_diff>
--- a/Microsoft Excel/Tanvir/Day 01 .xlsx
+++ b/Microsoft Excel/Tanvir/Day 01 .xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taroto/Documents/GitHub/Spreadsheet/Microsoft Excel/Tanvir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972B74FC-95A2-F74E-9D1D-1109BDB71095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B761F666-E747-204D-8E3B-DB451E474A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16100" xr2:uid="{3B72C934-E4E5-364A-A416-50801A8A56BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{3B72C934-E4E5-364A-A416-50801A8A56BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="DAY 01" sheetId="1" r:id="rId1"/>
+    <sheet name="17 Jan 2025" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DAY 01'!$K$3:$O$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'17 Jan 2025'!$K$3:$O$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">COPY </t>
   </si>
@@ -344,6 +344,21 @@
   </si>
   <si>
     <t>$B$2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addition </t>
+  </si>
+  <si>
+    <t xml:space="preserve">subtraction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiplication </t>
+  </si>
+  <si>
+    <t xml:space="preserve">divition </t>
+  </si>
+  <si>
+    <t>Not possible</t>
   </si>
 </sst>
 </file>
@@ -381,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,12 +406,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,12 +429,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -433,6 +436,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,21 +470,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -474,16 +486,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,7 +706,10 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
           <a:solidFill>
@@ -717,19 +740,98 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="2000" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
               <a:latin typeface="Arial Rounded MT Bold" panose="020F0704030504030204" pitchFamily="34" charset="77"/>
             </a:rPr>
             <a:t>Learning</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="2000" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
               <a:latin typeface="Arial Rounded MT Bold" panose="020F0704030504030204" pitchFamily="34" charset="77"/>
             </a:rPr>
             <a:t> Reference : Relative vs Absolute </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="2000" kern="1200">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
             <a:latin typeface="Arial Rounded MT Bold" panose="020F0704030504030204" pitchFamily="34" charset="77"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>710595</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>30238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>393095</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>120952</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7F87F7A-E580-3D1C-E8C0-267DE357D8AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11052024" y="2812143"/>
+          <a:ext cx="2388809" cy="483809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" kern="1200"/>
+            <a:t>OPERATIONS </a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1037,1190 +1139,1281 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2768DDA9-5909-8740-96D7-175223D96215}">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="8" customWidth="1"/>
     <col min="9" max="9" width="2.1640625" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
     </row>
     <row r="2" spans="1:24" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="10"/>
-      <c r="R2" s="14" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="R2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
         <v>2</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="K3" s="5" t="s">
+      <c r="I3" s="3"/>
+      <c r="K3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="R3" s="13" t="s">
+      <c r="P3" s="2"/>
+      <c r="R3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="S3" s="13">
+      <c r="S3" s="9">
         <v>11</v>
       </c>
-      <c r="T3" s="13">
+      <c r="T3" s="9">
         <f>$W$12*S3</f>
         <v>385</v>
       </c>
-      <c r="U3" s="13"/>
-      <c r="V3" s="15" t="s">
+      <c r="U3" s="9"/>
+      <c r="V3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="W3" s="15" t="s">
+      <c r="W3" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="X3" s="13"/>
+      <c r="X3" s="9"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="13">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="13">
         <v>4</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="6">
         <v>45659</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="2">
         <v>21</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="2">
         <v>0</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="2">
         <v>50000</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="2">
         <f>M4-N4</f>
         <v>-50000</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="R4" s="13" t="s">
+      <c r="P4" s="2"/>
+      <c r="R4" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="S4" s="13">
+      <c r="S4" s="9">
         <v>20</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="9">
         <f t="shared" ref="T4:T12" si="0">$W$12*S4</f>
         <v>700</v>
       </c>
-      <c r="U4" s="13"/>
-      <c r="V4" s="15" t="s">
+      <c r="U4" s="9"/>
+      <c r="V4" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="X4" s="13"/>
+      <c r="X4" s="9"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="13">
         <v>5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="13">
         <v>6</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="6">
         <v>45660</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="2">
         <v>21</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="2">
         <v>0</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2">
         <v>8000</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="2">
         <f t="shared" ref="O5:O9" si="1">M5-N5</f>
         <v>-8000</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="R5" s="13" t="s">
+      <c r="P5" s="2"/>
+      <c r="R5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="S5" s="13">
+      <c r="S5" s="9">
         <v>14</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="9">
         <f t="shared" si="0"/>
         <v>490</v>
       </c>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="13">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="13">
         <v>8</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="6">
         <v>45661</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="2">
         <v>22</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="2">
         <v>12000</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2">
         <v>9000</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="2">
         <f t="shared" si="1"/>
         <v>3000</v>
       </c>
-      <c r="P6" s="5"/>
-      <c r="R6" s="13" t="s">
+      <c r="P6" s="2"/>
+      <c r="R6" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="S6" s="13">
+      <c r="S6" s="9">
         <v>25</v>
       </c>
-      <c r="T6" s="13">
+      <c r="T6" s="9">
         <f t="shared" si="0"/>
         <v>875</v>
       </c>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="13">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="13">
         <v>10</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="6">
         <v>45662</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H7" t="s">
         <v>37</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="2">
         <v>22</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="2">
         <v>2000</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2">
         <v>2500</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="2">
         <f t="shared" si="1"/>
         <v>-500</v>
       </c>
-      <c r="P7" s="5"/>
-      <c r="R7" s="13" t="s">
+      <c r="P7" s="2"/>
+      <c r="R7" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="S7" s="13">
+      <c r="S7" s="9">
         <v>25</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="9">
         <f t="shared" si="0"/>
         <v>875</v>
       </c>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="13">
         <v>11</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="13">
         <v>12</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <v>45663</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="2">
         <v>22</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="2">
         <v>3000</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2">
         <v>1500</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="2">
         <f t="shared" si="1"/>
         <v>1500</v>
       </c>
-      <c r="P8" s="5"/>
-      <c r="R8" s="13" t="s">
+      <c r="P8" s="2"/>
+      <c r="R8" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="S8" s="13">
+      <c r="S8" s="9">
         <v>33</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="9">
         <f t="shared" si="0"/>
         <v>1155</v>
       </c>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="13">
         <v>13</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="13">
         <v>14</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="6">
         <v>45664</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="2">
         <v>21</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="2">
         <v>1000</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2">
         <v>1500</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="2">
         <f t="shared" si="1"/>
         <v>-500</v>
       </c>
-      <c r="P9" s="5"/>
-      <c r="R9" s="13" t="s">
+      <c r="P9" s="2"/>
+      <c r="R9" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S9" s="13">
+      <c r="S9" s="9">
         <v>7</v>
       </c>
-      <c r="T9" s="13">
+      <c r="T9" s="9">
         <f t="shared" si="0"/>
         <v>245</v>
       </c>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="13">
         <v>15</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="13">
         <v>16</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="6">
         <v>45665</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H10" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="R10" s="13" t="s">
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="R10" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S10" s="13">
+      <c r="S10" s="9">
         <v>14</v>
       </c>
-      <c r="T10" s="13">
+      <c r="T10" s="9">
         <f t="shared" si="0"/>
         <v>490</v>
       </c>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="13">
         <v>17</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="13">
         <v>18</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="6">
         <v>45666</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H11" t="s">
         <v>41</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="R11" s="13" t="s">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="R11" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="S11" s="13">
+      <c r="S11" s="9">
         <v>51</v>
       </c>
-      <c r="T11" s="13">
+      <c r="T11" s="9">
         <f t="shared" si="0"/>
         <v>1785</v>
       </c>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" s="13">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13">
         <v>10</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="13">
         <v>19</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="13">
         <v>20</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="6">
         <v>45667</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="R12" s="13" t="s">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="R12" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="S12" s="13">
+      <c r="S12" s="9">
         <v>22</v>
       </c>
-      <c r="T12" s="13">
+      <c r="T12" s="9">
         <f t="shared" si="0"/>
         <v>770</v>
       </c>
-      <c r="U12" s="13"/>
-      <c r="V12" s="15" t="s">
+      <c r="U12" s="9"/>
+      <c r="V12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="W12" s="15">
+      <c r="W12" s="11">
         <v>35</v>
       </c>
-      <c r="X12" s="13"/>
+      <c r="X12" s="9"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="A13" s="13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13">
         <v>11</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="13">
         <v>21</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="13">
         <v>22</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="6">
         <v>45668</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H13" t="s">
         <v>43</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="R13" s="13" t="s">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="R13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="S13" s="13">
+      <c r="S13" s="9">
         <v>32</v>
       </c>
-      <c r="T13" s="13">
+      <c r="T13" s="9">
         <f>$W$13*S13</f>
         <v>1280</v>
       </c>
-      <c r="U13" s="13"/>
-      <c r="V13" s="15" t="s">
+      <c r="U13" s="9"/>
+      <c r="V13" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="W13" s="15">
+      <c r="W13" s="11">
         <v>40</v>
       </c>
-      <c r="X13" s="13"/>
+      <c r="X13" s="9"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" s="13">
+        <v>1</v>
+      </c>
+      <c r="B14" s="13">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="13">
         <v>23</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="13">
         <v>24</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="6">
         <v>45669</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H14" t="s">
         <v>44</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="R14" s="13" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="R14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="S14" s="13">
+      <c r="S14" s="9">
         <v>23</v>
       </c>
-      <c r="T14" s="13">
+      <c r="T14" s="9">
         <f t="shared" ref="T14:T21" si="2">$W$13*S14</f>
         <v>920</v>
       </c>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" s="13">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13">
         <v>13</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="13">
         <v>25</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="13">
         <v>26</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="6">
         <v>45670</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H15" t="s">
         <v>45</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="R15" s="13" t="s">
+      <c r="K15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="R15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S15" s="13">
+      <c r="S15" s="9">
         <v>14</v>
       </c>
-      <c r="T15" s="13">
+      <c r="T15" s="9">
         <f t="shared" si="2"/>
         <v>560</v>
       </c>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1">
+      <c r="A16" s="13">
+        <v>1</v>
+      </c>
+      <c r="B16" s="13">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="13">
         <v>27</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="13">
         <v>28</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="6">
         <v>45671</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H16" t="s">
         <v>46</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="R16" s="13" t="s">
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <v>20</v>
+      </c>
+      <c r="M16" s="4">
+        <v>1</v>
+      </c>
+      <c r="N16" s="4">
+        <v>1000</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="R16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="S16" s="13">
+      <c r="S16" s="9">
         <v>41</v>
       </c>
-      <c r="T16" s="13">
+      <c r="T16" s="9">
         <f t="shared" si="2"/>
         <v>1640</v>
       </c>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1">
+      <c r="A17" s="13">
+        <v>1</v>
+      </c>
+      <c r="B17" s="13">
         <v>15</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="13">
         <v>29</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="13">
         <v>30</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="6">
         <v>45672</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H17" t="s">
         <v>47</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="R17" s="13" t="s">
+      <c r="K17" s="4">
+        <v>2</v>
+      </c>
+      <c r="L17" s="4">
+        <v>1</v>
+      </c>
+      <c r="M17" s="4">
+        <v>2</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="R17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="S17" s="13">
+      <c r="S17" s="9">
         <v>33</v>
       </c>
-      <c r="T17" s="13">
+      <c r="T17" s="9">
         <f t="shared" si="2"/>
         <v>1320</v>
       </c>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1">
+      <c r="A18" s="13">
+        <v>1</v>
+      </c>
+      <c r="B18" s="13">
         <v>16</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="13">
         <v>31</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="13">
         <v>32</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="6">
         <v>45673</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H18" t="s">
         <v>48</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="R18" s="13" t="s">
+      <c r="K18" s="4">
+        <v>5</v>
+      </c>
+      <c r="L18" s="4">
+        <v>2</v>
+      </c>
+      <c r="M18" s="4">
+        <v>3</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="R18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="S18" s="13">
+      <c r="S18" s="9">
         <v>64</v>
       </c>
-      <c r="T18" s="13">
+      <c r="T18" s="9">
         <f t="shared" si="2"/>
         <v>2560</v>
       </c>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="A19" s="13">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13">
         <v>17</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="13">
         <v>33</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="13">
         <v>34</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="6">
         <v>45674</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H19" t="s">
         <v>49</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="R19" s="13" t="s">
+      <c r="K19" s="4">
+        <v>3</v>
+      </c>
+      <c r="L19" s="4">
+        <v>3</v>
+      </c>
+      <c r="M19" s="4">
+        <v>4</v>
+      </c>
+      <c r="N19" s="4">
+        <v>2</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="R19" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="S19" s="13">
+      <c r="S19" s="9">
         <v>35</v>
       </c>
-      <c r="T19" s="13">
+      <c r="T19" s="9">
         <f t="shared" si="2"/>
         <v>1400</v>
       </c>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="A20" s="13">
+        <v>1</v>
+      </c>
+      <c r="B20" s="13">
         <v>18</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="13">
         <v>35</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="13">
         <v>36</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="6">
         <v>45675</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="8" t="s">
         <v>22</v>
       </c>
       <c r="H20" t="s">
         <v>50</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="R20" s="13" t="s">
+      <c r="K20" s="4">
+        <v>4</v>
+      </c>
+      <c r="L20" s="4">
+        <v>4</v>
+      </c>
+      <c r="M20" s="4">
+        <v>5</v>
+      </c>
+      <c r="N20" s="4">
+        <v>2</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="R20" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="S20" s="13">
+      <c r="S20" s="9">
         <v>44</v>
       </c>
-      <c r="T20" s="13">
+      <c r="T20" s="9">
         <f t="shared" si="2"/>
         <v>1760</v>
       </c>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1">
+      <c r="A21" s="13">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13">
         <v>19</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="13">
         <v>37</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="13">
         <v>38</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="6">
         <v>45676</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="8" t="s">
         <v>23</v>
       </c>
       <c r="H21" t="s">
         <v>51</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="R21" s="13" t="s">
+      <c r="K21" s="4">
+        <v>6</v>
+      </c>
+      <c r="L21" s="4">
+        <v>5</v>
+      </c>
+      <c r="M21" s="4">
+        <v>6</v>
+      </c>
+      <c r="N21" s="4">
+        <v>3</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="R21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="S21" s="13">
+      <c r="S21" s="9">
         <v>49</v>
       </c>
-      <c r="T21" s="13">
+      <c r="T21" s="9">
         <f t="shared" si="2"/>
         <v>1960</v>
       </c>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1">
+      <c r="A22" s="13">
+        <v>1</v>
+      </c>
+      <c r="B22" s="13">
         <v>20</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="13">
         <v>39</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="13">
         <v>40</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="6">
         <v>45677</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="8" t="s">
         <v>24</v>
       </c>
       <c r="H22" t="s">
         <v>52</v>
       </c>
       <c r="I22" s="1"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
+      <c r="K22" s="4">
+        <v>7</v>
+      </c>
+      <c r="L22" s="4">
+        <v>10</v>
+      </c>
+      <c r="M22" s="4">
+        <v>7</v>
+      </c>
+      <c r="N22" s="4">
+        <v>3</v>
+      </c>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1">
+      <c r="A23" s="13">
+        <v>1</v>
+      </c>
+      <c r="B23" s="13">
         <v>21</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="13">
         <v>41</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="13">
         <v>42</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="6">
         <v>45678</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="8" t="s">
         <v>25</v>
       </c>
       <c r="H23" t="s">
         <v>53</v>
       </c>
       <c r="I23" s="1"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
+      <c r="K23" s="4">
+        <v>8</v>
+      </c>
+      <c r="L23" s="4">
+        <v>2</v>
+      </c>
+      <c r="M23" s="4">
+        <v>8</v>
+      </c>
+      <c r="N23" s="4">
+        <v>4</v>
+      </c>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1">
+      <c r="A24" s="13">
+        <v>1</v>
+      </c>
+      <c r="B24" s="13">
         <v>22</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="13">
         <v>43</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="13">
         <v>44</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="6">
         <v>45679</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H24" t="s">
         <v>54</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
+      <c r="K24" s="4">
+        <v>9</v>
+      </c>
+      <c r="L24" s="4">
+        <v>2</v>
+      </c>
+      <c r="M24" s="4">
+        <v>9</v>
+      </c>
+      <c r="N24" s="4">
+        <v>4</v>
+      </c>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1">
+      <c r="A25" s="13">
+        <v>1</v>
+      </c>
+      <c r="B25" s="13">
         <v>23</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="13">
         <v>45</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="13">
         <v>46</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="6">
         <v>45680</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H25" t="s">
         <v>55</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
+      <c r="K25" s="4">
+        <f>K16+K17+K18+K20+K19+K21+K22+K23+K24</f>
+        <v>45</v>
+      </c>
+      <c r="L25" s="4">
+        <f>$L$16-L17-L18-L19-L20-L21-L23-L22-L24</f>
+        <v>-9</v>
+      </c>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1">
+      <c r="A26" s="13">
+        <v>1</v>
+      </c>
+      <c r="B26" s="13">
         <v>24</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="13">
         <v>47</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="13">
         <v>48</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="6">
         <v>45681</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="8" t="s">
         <v>28</v>
       </c>
       <c r="H26" t="s">
         <v>56</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
+      <c r="K26" s="4">
+        <f>SUM(K16:K24)</f>
+        <v>45</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1">
+      <c r="A27" s="13">
+        <v>1</v>
+      </c>
+      <c r="B27" s="13">
         <v>25</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="13">
         <v>49</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="13">
         <v>50</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="6">
         <v>45682</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H27" t="s">
         <v>57</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1">
+      <c r="A28" s="13">
+        <v>1</v>
+      </c>
+      <c r="B28" s="13">
         <v>26</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="13">
         <v>51</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="13">
         <v>52</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="6">
         <v>45683</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H28" t="s">
@@ -2229,22 +2422,22 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>1</v>
-      </c>
-      <c r="B29" s="1">
+      <c r="A29" s="13">
+        <v>1</v>
+      </c>
+      <c r="B29" s="13">
         <v>27</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="13">
         <v>53</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="13">
         <v>54</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="6">
         <v>45684</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="8" t="s">
         <v>31</v>
       </c>
       <c r="H29" t="s">
@@ -2253,22 +2446,22 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>1</v>
-      </c>
-      <c r="B30" s="1">
+      <c r="A30" s="13">
+        <v>1</v>
+      </c>
+      <c r="B30" s="13">
         <v>28</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="13">
         <v>55</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="13">
         <v>56</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="6">
         <v>45685</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H30" t="s">
@@ -2277,22 +2470,22 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1">
+      <c r="A31" s="13">
+        <v>1</v>
+      </c>
+      <c r="B31" s="13">
         <v>29</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="13">
         <v>57</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="13">
         <v>58</v>
       </c>
-      <c r="F31" s="9">
+      <c r="F31" s="6">
         <v>45686</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="8" t="s">
         <v>33</v>
       </c>
       <c r="H31" t="s">

</xml_diff>

<commit_message>
Learning few more things
</commit_message>
<xml_diff>
--- a/Microsoft Excel/Tanvir/Day 01 .xlsx
+++ b/Microsoft Excel/Tanvir/Day 01 .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taroto/Documents/GitHub/Spreadsheet/Microsoft Excel/Tanvir/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarato/Documents/GitHub/Spreadsheet/Microsoft Excel/Tanvir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B761F666-E747-204D-8E3B-DB451E474A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A2A083-A6E6-5248-8266-6828AA4C1E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{3B72C934-E4E5-364A-A416-50801A8A56BF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{3B72C934-E4E5-364A-A416-50801A8A56BF}"/>
   </bookViews>
   <sheets>
     <sheet name="17 Jan 2025" sheetId="1" r:id="rId1"/>

</xml_diff>